<commit_message>
bhumethali edit and chinimaya miss bora bass
</commit_message>
<xml_diff>
--- a/ofc/estimates/Baniyaa gaun/v.xlsx
+++ b/ofc/estimates/Baniyaa gaun/v.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="100">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -340,6 +340,9 @@
   </si>
   <si>
     <t xml:space="preserve">g/d k|sf/sf] Sn] / l;N6L df6f]df ;j} lsl;dsf] vGg] sfd </t>
+  </si>
+  <si>
+    <t>labour cost only</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -522,12 +525,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -691,6 +720,27 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -701,23 +751,26 @@
     <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -734,29 +787,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1398,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,113 +1454,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="80" t="s">
+      <c r="H6" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="73" t="s">
+      <c r="H7" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1566,7 +1601,7 @@
       <c r="A9" s="8">
         <v>1</v>
       </c>
-      <c r="B9" s="93" t="s">
+      <c r="B9" s="71" t="s">
         <v>98</v>
       </c>
       <c r="C9" s="10"/>
@@ -1681,7 +1716,9 @@
       <c r="H14" s="14"/>
       <c r="I14" s="13"/>
       <c r="J14" s="15"/>
-      <c r="K14" s="12"/>
+      <c r="K14" s="94" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
@@ -1706,13 +1743,11 @@
         <f>G15*I15</f>
         <v>14720</v>
       </c>
-      <c r="K15" s="12"/>
+      <c r="K15" s="95"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
-      <c r="B16" s="9" t="s">
-        <v>20</v>
-      </c>
+      <c r="B16" s="9"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
@@ -1720,15 +1755,16 @@
       <c r="G16" s="13"/>
       <c r="H16" s="14"/>
       <c r="I16" s="13"/>
-      <c r="J16" s="15">
-        <f>0.13*J15</f>
-        <v>1913.6000000000001</v>
-      </c>
+      <c r="J16" s="15"/>
       <c r="K16" s="12"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>3</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>94</v>
+      </c>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
@@ -1739,40 +1775,47 @@
       <c r="J17" s="15"/>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>3</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="15"/>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="41">
+        <f>2*(TRUNC(D14/1.5,0)+1)</f>
+        <v>22</v>
+      </c>
+      <c r="D18" s="18">
+        <v>6</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="19">
+        <f>PRODUCT(C18:F18)</f>
+        <v>132</v>
+      </c>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
       <c r="K18" s="12"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C19" s="41">
-        <f>2*(TRUNC(D14/1.5,0)+1)</f>
-        <v>22</v>
+        <f>3*2</f>
+        <v>6</v>
       </c>
       <c r="D19" s="18">
-        <v>6</v>
+        <f>D14</f>
+        <v>15</v>
       </c>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="19">
         <f>PRODUCT(C19:F19)</f>
-        <v>132</v>
+        <v>90</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="20"/>
@@ -1782,56 +1825,49 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="41">
-        <v>3</v>
-      </c>
-      <c r="D20" s="18">
-        <f>10</f>
-        <v>10</v>
-      </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="19">
-        <f>PRODUCT(C20:F20)</f>
-        <v>30</v>
-      </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
+        <v>18</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="13">
+        <f>(SUM(G18:G19))/6</f>
+        <v>37</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="13">
+        <v>240</v>
+      </c>
+      <c r="J20" s="15">
+        <f>G20*I20</f>
+        <v>8880</v>
+      </c>
       <c r="K20" s="12"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
-      <c r="G21" s="13">
-        <f>(SUM(G19:G20))/6</f>
-        <v>27</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="13">
-        <v>240</v>
-      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="15">
-        <f>G21*I21</f>
-        <v>6480</v>
+        <f>0.13*J20</f>
+        <v>1154.4000000000001</v>
       </c>
       <c r="K21" s="12"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
-      <c r="B22" s="9" t="s">
-        <v>20</v>
-      </c>
+      <c r="B22" s="9"/>
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
       <c r="E22" s="12"/>
@@ -1839,128 +1875,133 @@
       <c r="G22" s="13"/>
       <c r="H22" s="14"/>
       <c r="I22" s="13"/>
-      <c r="J22" s="15">
-        <f>0.13*J21</f>
-        <v>842.4</v>
-      </c>
+      <c r="J22" s="15"/>
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
+      <c r="A23" s="70">
+        <v>4</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="10">
+        <v>1</v>
+      </c>
       <c r="D23" s="11"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="15"/>
+      <c r="G23" s="30">
+        <f t="shared" ref="G23" si="0">PRODUCT(C23:F23)</f>
+        <v>1</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="13">
+        <v>500</v>
+      </c>
+      <c r="J23" s="30">
+        <f>G23*I23</f>
+        <v>500</v>
+      </c>
       <c r="K23" s="12"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="70">
-        <v>4</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="10">
-        <v>1</v>
-      </c>
+      <c r="A24" s="8"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
-      <c r="G24" s="30">
-        <f t="shared" ref="G24" si="0">PRODUCT(C24:F24)</f>
-        <v>1</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" s="13">
-        <v>500</v>
-      </c>
-      <c r="J24" s="30">
-        <f>G24*I24</f>
-        <v>500</v>
-      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="15"/>
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="12"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="41"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15">
+        <f>SUM(J9:J23)</f>
+        <v>84952.299999999988</v>
+      </c>
+      <c r="K25" s="17"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
-      <c r="B26" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15">
-        <f>SUM(J9:J24)</f>
-        <v>84153.9</v>
-      </c>
-      <c r="K26" s="17"/>
+      <c r="A26" s="60"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="64"/>
+      <c r="K26" s="65"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="60"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="64"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="65"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="78">
+        <f>J25</f>
+        <v>84952.299999999988</v>
+      </c>
+      <c r="D27" s="78"/>
+      <c r="E27" s="19">
+        <v>100</v>
+      </c>
+      <c r="F27" s="32"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="36"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="71">
-        <f>J26</f>
-        <v>84153.9</v>
-      </c>
-      <c r="D28" s="71"/>
-      <c r="E28" s="19">
-        <v>100</v>
-      </c>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="35"/>
-      <c r="K28" s="36"/>
+        <v>24</v>
+      </c>
+      <c r="C28" s="81">
+        <v>250000</v>
+      </c>
+      <c r="D28" s="81"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="38"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="74">
-        <v>250000</v>
-      </c>
-      <c r="D29" s="74"/>
-      <c r="E29" s="19"/>
+        <v>25</v>
+      </c>
+      <c r="C29" s="81">
+        <f>C28-C31-C32</f>
+        <v>237500</v>
+      </c>
+      <c r="D29" s="81"/>
+      <c r="E29" s="19">
+        <f>C29/C27*100</f>
+        <v>279.56865205532989</v>
+      </c>
       <c r="F29" s="38"/>
       <c r="G29" s="39"/>
       <c r="H29" s="39"/>
@@ -1971,16 +2012,16 @@
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="74">
-        <f>C29-C32-C33</f>
-        <v>237500</v>
-      </c>
-      <c r="D30" s="74"/>
+        <v>26</v>
+      </c>
+      <c r="C30" s="78">
+        <f>C27-C29</f>
+        <v>-152547.70000000001</v>
+      </c>
+      <c r="D30" s="78"/>
       <c r="E30" s="19">
-        <f>C30/C28*100</f>
-        <v>282.22102600117165</v>
+        <f>100-E29</f>
+        <v>-179.56865205532989</v>
       </c>
       <c r="F30" s="38"/>
       <c r="G30" s="39"/>
@@ -1992,16 +2033,15 @@
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="37"/>
       <c r="B31" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="71">
-        <f>C28-C30</f>
-        <v>-153346.1</v>
-      </c>
-      <c r="D31" s="71"/>
+        <v>27</v>
+      </c>
+      <c r="C31" s="78">
+        <f>C28*0.03</f>
+        <v>7500</v>
+      </c>
+      <c r="D31" s="78"/>
       <c r="E31" s="19">
-        <f>100-E30</f>
-        <v>-182.22102600117165</v>
+        <v>3</v>
       </c>
       <c r="F31" s="38"/>
       <c r="G31" s="39"/>
@@ -2013,15 +2053,15 @@
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="71">
-        <f>C29*0.03</f>
-        <v>7500</v>
-      </c>
-      <c r="D32" s="71"/>
+        <v>28</v>
+      </c>
+      <c r="C32" s="78">
+        <f>C28*0.02</f>
+        <v>5000</v>
+      </c>
+      <c r="D32" s="78"/>
       <c r="E32" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F32" s="38"/>
       <c r="G32" s="39"/>
@@ -2030,28 +2070,17 @@
       <c r="J32" s="39"/>
       <c r="K32" s="38"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="71">
-        <f>C29*0.02</f>
-        <v>5000</v>
-      </c>
-      <c r="D33" s="71"/>
-      <c r="E33" s="19">
-        <v>2</v>
-      </c>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="38"/>
-    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="K14:K15"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -2059,14 +2088,6 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2097,90 +2118,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
     </row>
     <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
     </row>
     <row r="3" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
     </row>
     <row r="4" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-      <c r="J5" s="85"/>
-      <c r="K5" s="85"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="93"/>
+      <c r="K5" s="93"/>
     </row>
     <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="42"/>
-      <c r="C6" s="81" t="e">
+      <c r="C6" s="89" t="e">
         <f>F31</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="82"/>
+      <c r="D6" s="90"/>
       <c r="E6" s="43"/>
       <c r="F6" s="42"/>
       <c r="G6" s="42"/>
@@ -2188,11 +2209,11 @@
         <v>32</v>
       </c>
       <c r="I6" s="42"/>
-      <c r="J6" s="81">
+      <c r="J6" s="89">
         <f>I31</f>
         <v>283710.37399446999</v>
       </c>
-      <c r="K6" s="82"/>
+      <c r="K6" s="90"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
@@ -2201,77 +2222,77 @@
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
       <c r="D7" s="44"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="I7" s="87" t="s">
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="I7" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="79" t="e">
+      <c r="A8" s="72" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="I8" s="88" t="s">
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="I8" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="88"/>
-      <c r="K8" s="88"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="87"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="89" t="e">
+      <c r="A9" s="88" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
-      <c r="I9" s="88" t="s">
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="I9" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="88"/>
-      <c r="K9" s="88"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="91" t="s">
+      <c r="C11" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="92" t="s">
+      <c r="D11" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92" t="s">
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="91" t="s">
+      <c r="H11" s="84"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="K11" s="90" t="s">
+      <c r="K11" s="82" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="91"/>
-      <c r="B12" s="91"/>
-      <c r="C12" s="91"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
       <c r="D12" s="45" t="s">
         <v>41</v>
       </c>
@@ -2290,8 +2311,8 @@
       <c r="I12" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="91"/>
-      <c r="K12" s="90"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="82"/>
     </row>
     <row r="13" spans="1:13" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="54" t="e">
@@ -2464,16 +2485,16 @@
     </row>
     <row r="18" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="54"/>
-      <c r="B18" s="53" t="str">
-        <f>Estimate!B16</f>
-        <v>VAT calculation</v>
+      <c r="B18" s="53" t="e">
+        <f>Estimate!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="C18" s="46"/>
       <c r="D18" s="46"/>
       <c r="E18" s="46"/>
-      <c r="F18" s="46">
-        <f>Estimate!J16</f>
-        <v>1913.6000000000001</v>
+      <c r="F18" s="46" t="e">
+        <f>Estimate!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="G18" s="46"/>
       <c r="H18" s="46"/>
@@ -2481,14 +2502,14 @@
         <f>Valuation!J22</f>
         <v>206.12342400000003</v>
       </c>
-      <c r="J18" s="47">
+      <c r="J18" s="47" t="e">
         <f>I18-F18</f>
-        <v>-1707.476576</v>
+        <v>#REF!</v>
       </c>
       <c r="K18" s="48"/>
-      <c r="M18" s="57">
+      <c r="M18" s="57" t="e">
         <f t="shared" si="0"/>
-        <v>2392</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="19" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2597,11 +2618,11 @@
     </row>
     <row r="23" spans="1:13" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="54">
-        <f>Estimate!A18</f>
+        <f>Estimate!A17</f>
         <v>3</v>
       </c>
       <c r="B23" s="56" t="str">
-        <f>Estimate!B18</f>
+        <f>Estimate!B17</f>
         <v>Providing and laying Bamboo for the protection all complete</v>
       </c>
       <c r="C23" s="46" t="e">
@@ -2645,15 +2666,15 @@
     <row r="24" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="54"/>
       <c r="B24" s="53" t="str">
-        <f>Estimate!B22</f>
+        <f>Estimate!B21</f>
         <v>VAT calculation</v>
       </c>
       <c r="C24" s="46"/>
       <c r="D24" s="46"/>
       <c r="E24" s="46"/>
       <c r="F24" s="46">
-        <f>Estimate!J22</f>
-        <v>842.4</v>
+        <f>Estimate!J21</f>
+        <v>1154.4000000000001</v>
       </c>
       <c r="G24" s="46"/>
       <c r="H24" s="46"/>
@@ -2663,12 +2684,12 @@
       </c>
       <c r="J24" s="47">
         <f>I24-F24</f>
-        <v>1005.4684482830002</v>
+        <v>693.46844828300004</v>
       </c>
       <c r="K24" s="48"/>
       <c r="M24" s="57">
         <f t="shared" si="0"/>
-        <v>1053</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2777,23 +2798,23 @@
     </row>
     <row r="29" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="54">
-        <f>Estimate!A24</f>
+        <f>Estimate!A23</f>
         <v>4</v>
       </c>
       <c r="B29" s="49" t="str">
-        <f>Estimate!B24</f>
+        <f>Estimate!B23</f>
         <v>Information board (सुचना पाटि)</v>
       </c>
       <c r="C29" s="46" t="str">
-        <f>Estimate!H24</f>
+        <f>Estimate!H23</f>
         <v>no.</v>
       </c>
       <c r="D29" s="46">
-        <f>Estimate!G24</f>
+        <f>Estimate!G23</f>
         <v>1</v>
       </c>
       <c r="E29" s="46">
-        <f>Estimate!I24</f>
+        <f>Estimate!I23</f>
         <v>500</v>
       </c>
       <c r="F29" s="46">
@@ -2874,6 +2895,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="I9:K9"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
@@ -2881,19 +2915,6 @@
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
     <mergeCell ref="J11:J12"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2930,113 +2951,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="80" t="s">
+      <c r="H6" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="73" t="s">
+      <c r="H7" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -3841,11 +3862,11 @@
       <c r="B46" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="71">
+      <c r="C46" s="78">
         <f>J44</f>
         <v>283710.37399446999</v>
       </c>
-      <c r="D46" s="71"/>
+      <c r="D46" s="78"/>
       <c r="E46" s="19">
         <v>100</v>
       </c>
@@ -3861,10 +3882,10 @@
       <c r="B47" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="74">
+      <c r="C47" s="81">
         <v>250000</v>
       </c>
-      <c r="D47" s="74"/>
+      <c r="D47" s="81"/>
       <c r="E47" s="19"/>
       <c r="F47" s="38"/>
       <c r="G47" s="39"/>
@@ -3878,11 +3899,11 @@
       <c r="B48" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="74">
+      <c r="C48" s="81">
         <f>C47-C50-C51</f>
         <v>237500</v>
       </c>
-      <c r="D48" s="74"/>
+      <c r="D48" s="81"/>
       <c r="E48" s="19">
         <f>C48/C46*100</f>
         <v>83.712131021556971</v>
@@ -3899,11 +3920,11 @@
       <c r="B49" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="71">
+      <c r="C49" s="78">
         <f>C46-C48</f>
         <v>46210.373994469992</v>
       </c>
-      <c r="D49" s="71"/>
+      <c r="D49" s="78"/>
       <c r="E49" s="19">
         <f>100-E48</f>
         <v>16.287868978443029</v>
@@ -3920,11 +3941,11 @@
       <c r="B50" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="71">
+      <c r="C50" s="78">
         <f>C47*0.03</f>
         <v>7500</v>
       </c>
-      <c r="D50" s="71"/>
+      <c r="D50" s="78"/>
       <c r="E50" s="19">
         <v>3</v>
       </c>
@@ -3940,11 +3961,11 @@
       <c r="B51" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C51" s="71">
+      <c r="C51" s="78">
         <f>C47*0.02</f>
         <v>5000</v>
       </c>
-      <c r="D51" s="71"/>
+      <c r="D51" s="78"/>
       <c r="E51" s="19">
         <v>2</v>
       </c>
@@ -3957,13 +3978,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="A7:F7"/>
@@ -3972,6 +3986,13 @@
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3985,7 +4006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>

</xml_diff>